<commit_message>
increasing test coverage to 100%
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/cell_modeling/simulation/multi_algorithm/Model-Simulation.xlsx
+++ b/intro_to_wc_modeling/cell_modeling/simulation/multi_algorithm/Model-Simulation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,11 +23,17 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Species!$A$1:$L$147</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Species!$A$1:$L$147</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Species!$A$1:$L$147</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$K$147</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$K$147</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$6</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="1093">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -3590,9 +3596,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3682,9 +3688,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3750,25 +3756,25 @@
   </sheetPr>
   <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B139" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
-      <selection pane="bottomRight" activeCell="A147" activeCellId="0" sqref="A147"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.63967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4104,8 +4110,14 @@
         <v>54</v>
       </c>
       <c r="C16" s="0"/>
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E16" s="1" t="n">
         <v>44.0095</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>29</v>
@@ -4566,8 +4578,14 @@
         <v>99</v>
       </c>
       <c r="C39" s="0"/>
+      <c r="D39" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E39" s="1" t="n">
         <v>1.0079</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>29</v>
@@ -6822,7 +6840,7 @@
   </sheetPr>
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -6833,15 +6851,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.74898785425101"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -11414,12 +11432,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.5263157894737"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="47.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -11564,9 +11582,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>